<commit_message>
Add Runway + Cartesia video generation system
GTME A/B testing framework for LinkedIn posts:
- Video + Voice (Runway + Cartesia Sonic-3)
- Video + Text Only (Runway)
- Text Post (control)

New files:
- scripts/generate_video.py: CLI for AI video generation
- docs/API_INTEGRATION.md: Runway/Cartesia API reference
- docs/VIDEO_WORKFLOW.md: Quick start for CEO/CTO demo
- .env.example: API key template
- requirements.txt: Python dependencies
- videos/runway/prompts/*.json: Style templates

Updated:
- build_tracker.py: Video tracking columns + dashboard
- Excel tracker: Video performance analytics section
- README.md: GTME-focused concise version
- .gitignore: Exclude generated videos

Runway: Gen-3 Alpha Turbo (text-to-video)
Cartesia: Sonic-3 with emotional tagging

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tracking/linkedin_engagement_tracker.xlsx
+++ b/tracking/linkedin_engagement_tracker.xlsx
@@ -18,9 +18,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.0&quot;%&quot;"/>
+    <numFmt numFmtId="166" formatCode="$0.00"/>
+    <numFmt numFmtId="167" formatCode="+0.0%;-0.0%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -42,7 +44,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -53,6 +55,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="004A90E2"/>
         <bgColor rgb="004A90E2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009B59B6"/>
+        <bgColor rgb="009B59B6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E74C3C"/>
+        <bgColor rgb="00E74C3C"/>
       </patternFill>
     </fill>
   </fills>
@@ -68,22 +82,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -113,6 +131,20 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="0034A853"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00E8D5E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00D5E8D5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -510,7 +542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -525,20 +557,24 @@
     <col width="20" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="10" customWidth="1" min="8" max="8"/>
-    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="35" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="35" customWidth="1" min="13" max="13"/>
+    <col width="8" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="8" customWidth="1" min="13" max="13"/>
     <col width="12" customWidth="1" min="14" max="14"/>
     <col width="12" customWidth="1" min="15" max="15"/>
     <col width="12" customWidth="1" min="16" max="16"/>
-    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="35" customWidth="1" min="17" max="17"/>
     <col width="12" customWidth="1" min="18" max="18"/>
     <col width="12" customWidth="1" min="19" max="19"/>
-    <col width="15" customWidth="1" min="20" max="20"/>
+    <col width="12" customWidth="1" min="20" max="20"/>
+    <col width="12" customWidth="1" min="21" max="21"/>
+    <col width="12" customWidth="1" min="22" max="22"/>
+    <col width="12" customWidth="1" min="23" max="23"/>
+    <col width="15" customWidth="1" min="24" max="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -569,75 +605,95 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Video Type</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Video Style</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Video URL</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Video Cost</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Impressions</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Likes</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Comments</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Shares</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>DMs Received</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Videos Sent</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Demos Booked</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Total Engagement</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Engagement %</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Conversion %</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Video→Demo %</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Cost/Engage</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Tier</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -667,57 +723,76 @@
           <t>Hand-Raiser</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Runway</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Pain Point Illustration</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://app.runwayml.com/video/ec001</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J2" t="n">
         <v>1247</v>
       </c>
-      <c r="G2" t="n">
+      <c r="K2" t="n">
         <v>63</v>
       </c>
-      <c r="H2" t="n">
+      <c r="L2" t="n">
         <v>8</v>
       </c>
-      <c r="I2" t="n">
+      <c r="M2" t="n">
         <v>2</v>
       </c>
-      <c r="J2" t="n">
+      <c r="N2" t="n">
         <v>5</v>
       </c>
-      <c r="K2" t="n">
+      <c r="O2" t="n">
         <v>5</v>
       </c>
-      <c r="L2" t="n">
+      <c r="P2" t="n">
         <v>2</v>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>High engagement on copper price spike</t>
-        </is>
-      </c>
-      <c r="N2">
-        <f>SUM(G2:I2)</f>
-        <v/>
-      </c>
-      <c r="O2" s="3">
-        <f>IF(F2&gt;0,N2/F2*100,0)</f>
-        <v/>
-      </c>
-      <c r="P2" s="3">
-        <f>IF(F2&gt;0,(H2+J2)/F2*100,0)</f>
-        <v/>
-      </c>
-      <c r="Q2" s="3">
-        <f>IF(K2&gt;0,L2/K2*100,0)</f>
-        <v/>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <f>IF(O2&gt;=5,"🟢 High",IF(O2&gt;=2,"🟡 Medium","🔴 Low"))</f>
-        <v/>
-      </c>
-      <c r="T2">
-        <f>IF(L2&gt;0,"✅ Closed",IF(K2&gt;0,"📹 Video Sent",IF(J2&gt;0,"💬 Engaged","👀 Posted")))</f>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Runway video: copper price spike animation - high engagement</t>
+        </is>
+      </c>
+      <c r="R2">
+        <f>SUM(K2:M2)</f>
+        <v/>
+      </c>
+      <c r="S2" s="3">
+        <f>IF(J2&gt;0,R2/J2*100,0)</f>
+        <v/>
+      </c>
+      <c r="T2" s="3">
+        <f>IF(J2&gt;0,(L2+N2)/J2*100,0)</f>
+        <v/>
+      </c>
+      <c r="U2" s="3">
+        <f>IF(O2&gt;0,P2/O2*100,0)</f>
+        <v/>
+      </c>
+      <c r="V2" s="4">
+        <f>IF(R2&gt;0,I2/R2,0)</f>
+        <v/>
+      </c>
+      <c r="W2">
+        <f>IF(S2&gt;=5,"🟢 High",IF(S2&gt;=2,"🟡 Medium","🔴 Low"))</f>
+        <v/>
+      </c>
+      <c r="X2">
+        <f>IF(P2&gt;0,"✅ Closed",IF(O2&gt;0,"📹 Video Sent",IF(N2&gt;0,"💬 Engaged","👀 Posted")))</f>
         <v/>
       </c>
     </row>
@@ -737,7 +812,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Labor Burden</t>
+          <t>Labor Burden Blindness</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -745,57 +820,72 @@
           <t>Hand-Raiser</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
         <v>892</v>
       </c>
-      <c r="G3" t="n">
+      <c r="K3" t="n">
         <v>34</v>
       </c>
-      <c r="H3" t="n">
+      <c r="L3" t="n">
         <v>3</v>
       </c>
-      <c r="I3" t="n">
+      <c r="M3" t="n">
         <v>1</v>
       </c>
-      <c r="J3" t="n">
+      <c r="N3" t="n">
         <v>2</v>
       </c>
-      <c r="K3" t="n">
+      <c r="O3" t="n">
         <v>2</v>
       </c>
-      <c r="L3" t="n">
+      <c r="P3" t="n">
         <v>0</v>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Lower engagement, may need refinement</t>
-        </is>
-      </c>
-      <c r="N3">
-        <f>SUM(G3:I3)</f>
-        <v/>
-      </c>
-      <c r="O3" s="3">
-        <f>IF(F3&gt;0,N3/F3*100,0)</f>
-        <v/>
-      </c>
-      <c r="P3" s="3">
-        <f>IF(F3&gt;0,(H3+J3)/F3*100,0)</f>
-        <v/>
-      </c>
-      <c r="Q3" s="3">
-        <f>IF(K3&gt;0,L3/K3*100,0)</f>
-        <v/>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <f>IF(O3&gt;=5,"🟢 High",IF(O3&gt;=2,"🟡 Medium","🔴 Low"))</f>
-        <v/>
-      </c>
-      <c r="T3">
-        <f>IF(L3&gt;0,"✅ Closed",IF(K3&gt;0,"📹 Video Sent",IF(J3&gt;0,"💬 Engaged","👀 Posted")))</f>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Text-only baseline test for comparison</t>
+        </is>
+      </c>
+      <c r="R3">
+        <f>SUM(K3:M3)</f>
+        <v/>
+      </c>
+      <c r="S3" s="3">
+        <f>IF(J3&gt;0,R3/J3*100,0)</f>
+        <v/>
+      </c>
+      <c r="T3" s="3">
+        <f>IF(J3&gt;0,(L3+N3)/J3*100,0)</f>
+        <v/>
+      </c>
+      <c r="U3" s="3">
+        <f>IF(O3&gt;0,P3/O3*100,0)</f>
+        <v/>
+      </c>
+      <c r="V3" s="4">
+        <f>IF(R3&gt;0,I3/R3,0)</f>
+        <v/>
+      </c>
+      <c r="W3">
+        <f>IF(S3&gt;=5,"🟢 High",IF(S3&gt;=2,"🟡 Medium","🔴 Low"))</f>
+        <v/>
+      </c>
+      <c r="X3">
+        <f>IF(P3&gt;0,"✅ Closed",IF(O3&gt;0,"📹 Video Sent",IF(N3&gt;0,"💬 Engaged","👀 Posted")))</f>
         <v/>
       </c>
     </row>
@@ -823,57 +913,76 @@
           <t>Hand-Raiser</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Loom</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Personal Demo</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://loom.com/share/hv001demo</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
         <v>1583</v>
       </c>
-      <c r="G4" t="n">
+      <c r="K4" t="n">
         <v>87</v>
       </c>
-      <c r="H4" t="n">
+      <c r="L4" t="n">
         <v>12</v>
       </c>
-      <c r="I4" t="n">
+      <c r="M4" t="n">
         <v>4</v>
       </c>
-      <c r="J4" t="n">
+      <c r="N4" t="n">
         <v>8</v>
       </c>
-      <c r="K4" t="n">
+      <c r="O4" t="n">
         <v>7</v>
       </c>
-      <c r="L4" t="n">
+      <c r="P4" t="n">
         <v>3</v>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Strong resonance on "80% done" angle</t>
-        </is>
-      </c>
-      <c r="N4">
-        <f>SUM(G4:I4)</f>
-        <v/>
-      </c>
-      <c r="O4" s="3">
-        <f>IF(F4&gt;0,N4/F4*100,0)</f>
-        <v/>
-      </c>
-      <c r="P4" s="3">
-        <f>IF(F4&gt;0,(H4+J4)/F4*100,0)</f>
-        <v/>
-      </c>
-      <c r="Q4" s="3">
-        <f>IF(K4&gt;0,L4/K4*100,0)</f>
-        <v/>
-      </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <f>IF(O4&gt;=5,"🟢 High",IF(O4&gt;=2,"🟡 Medium","🔴 Low"))</f>
-        <v/>
-      </c>
-      <c r="T4">
-        <f>IF(L4&gt;0,"✅ Closed",IF(K4&gt;0,"📹 Video Sent",IF(J4&gt;0,"💬 Engaged","👀 Posted")))</f>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Personal Loom explanation - strong resonance on "80% done"</t>
+        </is>
+      </c>
+      <c r="R4">
+        <f>SUM(K4:M4)</f>
+        <v/>
+      </c>
+      <c r="S4" s="3">
+        <f>IF(J4&gt;0,R4/J4*100,0)</f>
+        <v/>
+      </c>
+      <c r="T4" s="3">
+        <f>IF(J4&gt;0,(L4+N4)/J4*100,0)</f>
+        <v/>
+      </c>
+      <c r="U4" s="3">
+        <f>IF(O4&gt;0,P4/O4*100,0)</f>
+        <v/>
+      </c>
+      <c r="V4" s="4">
+        <f>IF(R4&gt;0,I4/R4,0)</f>
+        <v/>
+      </c>
+      <c r="W4">
+        <f>IF(S4&gt;=5,"🟢 High",IF(S4&gt;=2,"🟡 Medium","🔴 Low"))</f>
+        <v/>
+      </c>
+      <c r="X4">
+        <f>IF(P4&gt;0,"✅ Closed",IF(O4&gt;0,"📹 Video Sent",IF(N4&gt;0,"💬 Engaged","👀 Posted")))</f>
         <v/>
       </c>
     </row>
@@ -901,57 +1010,76 @@
           <t>Hand-Raiser</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Runway</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Text Overlay</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://app.runwayml.com/video/pl001</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="J5" t="n">
         <v>1129</v>
       </c>
-      <c r="G5" t="n">
+      <c r="K5" t="n">
         <v>56</v>
       </c>
-      <c r="H5" t="n">
+      <c r="L5" t="n">
         <v>6</v>
       </c>
-      <c r="I5" t="n">
+      <c r="M5" t="n">
         <v>2</v>
       </c>
-      <c r="J5" t="n">
+      <c r="N5" t="n">
         <v>4</v>
       </c>
-      <c r="K5" t="n">
+      <c r="O5" t="n">
         <v>4</v>
       </c>
-      <c r="L5" t="n">
+      <c r="P5" t="n">
         <v>1</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Office manager empathy angle worked</t>
-        </is>
-      </c>
-      <c r="N5">
-        <f>SUM(G5:I5)</f>
-        <v/>
-      </c>
-      <c r="O5" s="3">
-        <f>IF(F5&gt;0,N5/F5*100,0)</f>
-        <v/>
-      </c>
-      <c r="P5" s="3">
-        <f>IF(F5&gt;0,(H5+J5)/F5*100,0)</f>
-        <v/>
-      </c>
-      <c r="Q5" s="3">
-        <f>IF(K5&gt;0,L5/K5*100,0)</f>
-        <v/>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <f>IF(O5&gt;=5,"🟢 High",IF(O5&gt;=2,"🟡 Medium","🔴 Low"))</f>
-        <v/>
-      </c>
-      <c r="T5">
-        <f>IF(L5&gt;0,"✅ Closed",IF(K5&gt;0,"📹 Video Sent",IF(J5&gt;0,"💬 Engaged","👀 Posted")))</f>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Runway text animation: "3 HOURS A DAY" - office manager empathy</t>
+        </is>
+      </c>
+      <c r="R5">
+        <f>SUM(K5:M5)</f>
+        <v/>
+      </c>
+      <c r="S5" s="3">
+        <f>IF(J5&gt;0,R5/J5*100,0)</f>
+        <v/>
+      </c>
+      <c r="T5" s="3">
+        <f>IF(J5&gt;0,(L5+N5)/J5*100,0)</f>
+        <v/>
+      </c>
+      <c r="U5" s="3">
+        <f>IF(O5&gt;0,P5/O5*100,0)</f>
+        <v/>
+      </c>
+      <c r="V5" s="4">
+        <f>IF(R5&gt;0,I5/R5,0)</f>
+        <v/>
+      </c>
+      <c r="W5">
+        <f>IF(S5&gt;=5,"🟢 High",IF(S5&gt;=2,"🟡 Medium","🔴 Low"))</f>
+        <v/>
+      </c>
+      <c r="X5">
+        <f>IF(P5&gt;0,"✅ Closed",IF(O5&gt;0,"📹 Video Sent",IF(N5&gt;0,"💬 Engaged","👀 Posted")))</f>
         <v/>
       </c>
     </row>
@@ -979,57 +1107,76 @@
           <t>Hand-Raiser</t>
         </is>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Runway</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Abstract Motion</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>https://app.runwayml.com/video/hv002</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
         <v>743</v>
       </c>
-      <c r="G6" t="n">
+      <c r="K6" t="n">
         <v>28</v>
       </c>
-      <c r="H6" t="n">
+      <c r="L6" t="n">
         <v>2</v>
       </c>
-      <c r="I6" t="n">
+      <c r="M6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" t="n">
+      <c r="N6" t="n">
         <v>1</v>
       </c>
-      <c r="K6" t="n">
+      <c r="O6" t="n">
         <v>1</v>
       </c>
-      <c r="L6" t="n">
+      <c r="P6" t="n">
         <v>0</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Cross-tested electrical pain point, lower fit</t>
-        </is>
-      </c>
-      <c r="N6">
-        <f>SUM(G6:I6)</f>
-        <v/>
-      </c>
-      <c r="O6" s="3">
-        <f>IF(F6&gt;0,N6/F6*100,0)</f>
-        <v/>
-      </c>
-      <c r="P6" s="3">
-        <f>IF(F6&gt;0,(H6+J6)/F6*100,0)</f>
-        <v/>
-      </c>
-      <c r="Q6" s="3">
-        <f>IF(K6&gt;0,L6/K6*100,0)</f>
-        <v/>
-      </c>
-      <c r="R6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <f>IF(O6&gt;=5,"🟢 High",IF(O6&gt;=2,"🟡 Medium","🔴 Low"))</f>
-        <v/>
-      </c>
-      <c r="T6">
-        <f>IF(L6&gt;0,"✅ Closed",IF(K6&gt;0,"📹 Video Sent",IF(J6&gt;0,"💬 Engaged","👀 Posted")))</f>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Abstract motion graphics - lower fit for HVAC audience</t>
+        </is>
+      </c>
+      <c r="R6">
+        <f>SUM(K6:M6)</f>
+        <v/>
+      </c>
+      <c r="S6" s="3">
+        <f>IF(J6&gt;0,R6/J6*100,0)</f>
+        <v/>
+      </c>
+      <c r="T6" s="3">
+        <f>IF(J6&gt;0,(L6+N6)/J6*100,0)</f>
+        <v/>
+      </c>
+      <c r="U6" s="3">
+        <f>IF(O6&gt;0,P6/O6*100,0)</f>
+        <v/>
+      </c>
+      <c r="V6" s="4">
+        <f>IF(R6&gt;0,I6/R6,0)</f>
+        <v/>
+      </c>
+      <c r="W6">
+        <f>IF(S6&gt;=5,"🟢 High",IF(S6&gt;=2,"🟡 Medium","🔴 Low"))</f>
+        <v/>
+      </c>
+      <c r="X6">
+        <f>IF(P6&gt;0,"✅ Closed",IF(O6&gt;0,"📹 Video Sent",IF(N6&gt;0,"💬 Engaged","👀 Posted")))</f>
         <v/>
       </c>
     </row>
@@ -1057,62 +1204,77 @@
           <t>Educational</t>
         </is>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
         <v>1034</v>
       </c>
-      <c r="G7" t="n">
+      <c r="K7" t="n">
         <v>41</v>
       </c>
-      <c r="H7" t="n">
+      <c r="L7" t="n">
         <v>5</v>
       </c>
-      <c r="I7" t="n">
+      <c r="M7" t="n">
         <v>1</v>
       </c>
-      <c r="J7" t="n">
+      <c r="N7" t="n">
         <v>3</v>
       </c>
-      <c r="K7" t="n">
+      <c r="O7" t="n">
         <v>3</v>
       </c>
-      <c r="L7" t="n">
+      <c r="P7" t="n">
         <v>1</v>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>Testing new pain point angle</t>
-        </is>
-      </c>
-      <c r="N7">
-        <f>SUM(G7:I7)</f>
-        <v/>
-      </c>
-      <c r="O7" s="3">
-        <f>IF(F7&gt;0,N7/F7*100,0)</f>
-        <v/>
-      </c>
-      <c r="P7" s="3">
-        <f>IF(F7&gt;0,(H7+J7)/F7*100,0)</f>
-        <v/>
-      </c>
-      <c r="Q7" s="3">
-        <f>IF(K7&gt;0,L7/K7*100,0)</f>
-        <v/>
-      </c>
-      <c r="R7" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <f>IF(O7&gt;=5,"🟢 High",IF(O7&gt;=2,"🟡 Medium","🔴 Low"))</f>
-        <v/>
-      </c>
-      <c r="T7">
-        <f>IF(L7&gt;0,"✅ Closed",IF(K7&gt;0,"📹 Video Sent",IF(J7&gt;0,"💬 Engaged","👀 Posted")))</f>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Testing new pain point angle without video</t>
+        </is>
+      </c>
+      <c r="R7">
+        <f>SUM(K7:M7)</f>
+        <v/>
+      </c>
+      <c r="S7" s="3">
+        <f>IF(J7&gt;0,R7/J7*100,0)</f>
+        <v/>
+      </c>
+      <c r="T7" s="3">
+        <f>IF(J7&gt;0,(L7+N7)/J7*100,0)</f>
+        <v/>
+      </c>
+      <c r="U7" s="3">
+        <f>IF(O7&gt;0,P7/O7*100,0)</f>
+        <v/>
+      </c>
+      <c r="V7" s="4">
+        <f>IF(R7&gt;0,I7/R7,0)</f>
+        <v/>
+      </c>
+      <c r="W7">
+        <f>IF(S7&gt;=5,"🟢 High",IF(S7&gt;=2,"🟡 Medium","🔴 Low"))</f>
+        <v/>
+      </c>
+      <c r="X7">
+        <f>IF(P7&gt;0,"✅ Closed",IF(O7&gt;0,"📹 Video Sent",IF(N7&gt;0,"💬 Engaged","👀 Posted")))</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O2:O100">
+  <conditionalFormatting sqref="S2:S100">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1124,7 +1286,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S100">
+  <conditionalFormatting sqref="W2:W100">
     <cfRule type="cellIs" priority="2" operator="containsText" dxfId="0">
       <formula>"High"</formula>
     </cfRule>
@@ -1135,12 +1297,20 @@
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L100">
+  <conditionalFormatting sqref="P2:P100">
     <cfRule type="cellIs" priority="5" operator="greaterThan" dxfId="3">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <conditionalFormatting sqref="F2:F100">
+    <cfRule type="cellIs" priority="6" operator="containsText" dxfId="4">
+      <formula>"Runway"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="containsText" dxfId="5">
+      <formula>"Loom"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="5">
     <dataValidation sqref="C2:C100" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Electrical,HVAC,Plumbing,Energy,Multi-Vertical"</formula1>
     </dataValidation>
@@ -1149,6 +1319,12 @@
     </dataValidation>
     <dataValidation sqref="E2:E100" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Hand-Raiser,Educational,Case Study,Poll/Survey,Testimonial"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F100" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"None,Loom,Runway"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G100" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"N/A,Personal Demo,Abstract Motion,Pain Point Illustration,Text Overlay,Before-After"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1161,7 +1337,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1178,39 +1354,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>VERTICAL PERFORMANCE SUMMARY</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Vertical</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Total Posts</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>Avg Engage%</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
         <is>
           <t>Total DMs</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>Videos Sent</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>Demos Booked</t>
         </is>
@@ -1227,19 +1403,19 @@
         <v/>
       </c>
       <c r="C3" s="3">
-        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!C:C,"Electrical",'Post Performance Tracker'!O:O),0)</f>
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!C:C,"Electrical",'Post Performance Tracker'!S:S),0)</f>
         <v/>
       </c>
       <c r="D3">
-        <f>SUMIF('Post Performance Tracker'!C:C,"Electrical",'Post Performance Tracker'!J:J)</f>
+        <f>SUMIF('Post Performance Tracker'!C:C,"Electrical",'Post Performance Tracker'!N:N)</f>
         <v/>
       </c>
       <c r="E3">
-        <f>SUMIF('Post Performance Tracker'!C:C,"Electrical",'Post Performance Tracker'!K:K)</f>
+        <f>SUMIF('Post Performance Tracker'!C:C,"Electrical",'Post Performance Tracker'!O:O)</f>
         <v/>
       </c>
       <c r="F3">
-        <f>SUMIF('Post Performance Tracker'!C:C,"Electrical",'Post Performance Tracker'!L:L)</f>
+        <f>SUMIF('Post Performance Tracker'!C:C,"Electrical",'Post Performance Tracker'!P:P)</f>
         <v/>
       </c>
     </row>
@@ -1254,19 +1430,19 @@
         <v/>
       </c>
       <c r="C4" s="3">
-        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!C:C,"HVAC",'Post Performance Tracker'!O:O),0)</f>
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!C:C,"HVAC",'Post Performance Tracker'!S:S),0)</f>
         <v/>
       </c>
       <c r="D4">
-        <f>SUMIF('Post Performance Tracker'!C:C,"HVAC",'Post Performance Tracker'!J:J)</f>
+        <f>SUMIF('Post Performance Tracker'!C:C,"HVAC",'Post Performance Tracker'!N:N)</f>
         <v/>
       </c>
       <c r="E4">
-        <f>SUMIF('Post Performance Tracker'!C:C,"HVAC",'Post Performance Tracker'!K:K)</f>
+        <f>SUMIF('Post Performance Tracker'!C:C,"HVAC",'Post Performance Tracker'!O:O)</f>
         <v/>
       </c>
       <c r="F4">
-        <f>SUMIF('Post Performance Tracker'!C:C,"HVAC",'Post Performance Tracker'!L:L)</f>
+        <f>SUMIF('Post Performance Tracker'!C:C,"HVAC",'Post Performance Tracker'!P:P)</f>
         <v/>
       </c>
     </row>
@@ -1281,299 +1457,531 @@
         <v/>
       </c>
       <c r="C5" s="3">
-        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!C:C,"Plumbing",'Post Performance Tracker'!O:O),0)</f>
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!C:C,"Plumbing",'Post Performance Tracker'!S:S),0)</f>
         <v/>
       </c>
       <c r="D5">
-        <f>SUMIF('Post Performance Tracker'!C:C,"Plumbing",'Post Performance Tracker'!J:J)</f>
+        <f>SUMIF('Post Performance Tracker'!C:C,"Plumbing",'Post Performance Tracker'!N:N)</f>
         <v/>
       </c>
       <c r="E5">
-        <f>SUMIF('Post Performance Tracker'!C:C,"Plumbing",'Post Performance Tracker'!K:K)</f>
+        <f>SUMIF('Post Performance Tracker'!C:C,"Plumbing",'Post Performance Tracker'!O:O)</f>
         <v/>
       </c>
       <c r="F5">
-        <f>SUMIF('Post Performance Tracker'!C:C,"Plumbing",'Post Performance Tracker'!L:L)</f>
+        <f>SUMIF('Post Performance Tracker'!C:C,"Plumbing",'Post Performance Tracker'!P:P)</f>
         <v/>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <f>SUM(B3:B5)</f>
         <v/>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="8">
         <f>AVERAGE(C3:C5)</f>
         <v/>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <f>SUM(D3:D5)</f>
         <v/>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <f>SUM(E3:E5)</f>
         <v/>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="7">
         <f>SUM(F3:F5)</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>PAIN POINT PERFORMANCE</t>
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>VIDEO PERFORMANCE ANALYSIS</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>Pain Point</t>
-        </is>
-      </c>
-      <c r="B10" s="5" t="inlineStr">
-        <is>
-          <t>Posts Count</t>
-        </is>
-      </c>
-      <c r="C10" s="5" t="inlineStr">
+      <c r="A10" s="9" t="inlineStr">
+        <is>
+          <t>Video Type</t>
+        </is>
+      </c>
+      <c r="B10" s="9" t="inlineStr">
+        <is>
+          <t>Posts</t>
+        </is>
+      </c>
+      <c r="C10" s="9" t="inlineStr">
         <is>
           <t>Avg Engage%</t>
         </is>
       </c>
-      <c r="D10" s="5" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
+        <is>
+          <t>Total DMs</t>
+        </is>
+      </c>
+      <c r="E10" s="9" t="inlineStr">
         <is>
           <t>Demos</t>
+        </is>
+      </c>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>Lift vs None</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Material Cost Overruns</t>
+          <t>None</t>
         </is>
       </c>
       <c r="B11">
-        <f>COUNTIF('Post Performance Tracker'!D:D,"Material Cost Overruns")</f>
+        <f>COUNTIF('Post Performance Tracker'!F:F,"None")</f>
         <v/>
       </c>
       <c r="C11" s="3">
-        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!D:D,"Material Cost Overruns",'Post Performance Tracker'!O:O),0)</f>
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!F:F,"None",'Post Performance Tracker'!S:S),0)</f>
         <v/>
       </c>
       <c r="D11">
-        <f>SUMIF('Post Performance Tracker'!D:D,"Material Cost Overruns",'Post Performance Tracker'!L:L)</f>
-        <v/>
+        <f>SUMIF('Post Performance Tracker'!F:F,"None",'Post Performance Tracker'!N:N)</f>
+        <v/>
+      </c>
+      <c r="E11">
+        <f>SUMIF('Post Performance Tracker'!F:F,"None",'Post Performance Tracker'!P:P)</f>
+        <v/>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Labor Burden Blindness</t>
+          <t>Loom</t>
         </is>
       </c>
       <c r="B12">
-        <f>COUNTIF('Post Performance Tracker'!D:D,"Labor Burden Blindness")</f>
+        <f>COUNTIF('Post Performance Tracker'!F:F,"Loom")</f>
         <v/>
       </c>
       <c r="C12" s="3">
-        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!D:D,"Labor Burden Blindness",'Post Performance Tracker'!O:O),0)</f>
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!F:F,"Loom",'Post Performance Tracker'!S:S),0)</f>
         <v/>
       </c>
       <c r="D12">
-        <f>SUMIF('Post Performance Tracker'!D:D,"Labor Burden Blindness",'Post Performance Tracker'!L:L)</f>
+        <f>SUMIF('Post Performance Tracker'!F:F,"Loom",'Post Performance Tracker'!N:N)</f>
+        <v/>
+      </c>
+      <c r="E12">
+        <f>SUMIF('Post Performance Tracker'!F:F,"Loom",'Post Performance Tracker'!P:P)</f>
+        <v/>
+      </c>
+      <c r="F12" s="10">
+        <f>IF(C11&gt;0,C12/C11-1,0)</f>
         <v/>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Admin Time Waste</t>
+          <t>Runway</t>
         </is>
       </c>
       <c r="B13">
-        <f>COUNTIF('Post Performance Tracker'!D:D,"Admin Time Waste")</f>
+        <f>COUNTIF('Post Performance Tracker'!F:F,"Runway")</f>
         <v/>
       </c>
       <c r="C13" s="3">
-        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!D:D,"Admin Time Waste",'Post Performance Tracker'!O:O),0)</f>
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!F:F,"Runway",'Post Performance Tracker'!S:S),0)</f>
         <v/>
       </c>
       <c r="D13">
-        <f>SUMIF('Post Performance Tracker'!D:D,"Admin Time Waste",'Post Performance Tracker'!L:L)</f>
+        <f>SUMIF('Post Performance Tracker'!F:F,"Runway",'Post Performance Tracker'!N:N)</f>
+        <v/>
+      </c>
+      <c r="E13">
+        <f>SUMIF('Post Performance Tracker'!F:F,"Runway",'Post Performance Tracker'!P:P)</f>
+        <v/>
+      </c>
+      <c r="F13" s="10">
+        <f>IF(C11&gt;0,C13/C11-1,0)</f>
         <v/>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>WEEKLY TRENDS</t>
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>RUNWAY VIDEO STYLE PERFORMANCE</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="inlineStr">
-        <is>
-          <t>Week</t>
-        </is>
-      </c>
-      <c r="B17" s="5" t="inlineStr">
-        <is>
-          <t>Posts Published</t>
-        </is>
-      </c>
-      <c r="C17" s="5" t="inlineStr">
-        <is>
-          <t>Total DMs</t>
-        </is>
-      </c>
-      <c r="D17" s="5" t="inlineStr">
-        <is>
-          <t>Demos Booked</t>
+      <c r="A17" s="11" t="inlineStr">
+        <is>
+          <t>Video Style</t>
+        </is>
+      </c>
+      <c r="B17" s="11" t="inlineStr">
+        <is>
+          <t>Posts</t>
+        </is>
+      </c>
+      <c r="C17" s="11" t="inlineStr">
+        <is>
+          <t>Avg Engage%</t>
+        </is>
+      </c>
+      <c r="D17" s="11" t="inlineStr">
+        <is>
+          <t>DMs</t>
+        </is>
+      </c>
+      <c r="E17" s="11" t="inlineStr">
+        <is>
+          <t>Demos</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Week 1</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
+          <t>Abstract Motion</t>
+        </is>
+      </c>
+      <c r="B18">
+        <f>COUNTIF('Post Performance Tracker'!G:G,"Abstract Motion")</f>
+        <v/>
+      </c>
+      <c r="C18" s="3">
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!G:G,"Abstract Motion",'Post Performance Tracker'!S:S),0)</f>
+        <v/>
+      </c>
+      <c r="D18">
+        <f>SUMIF('Post Performance Tracker'!G:G,"Abstract Motion",'Post Performance Tracker'!N:N)</f>
+        <v/>
+      </c>
+      <c r="E18">
+        <f>SUMIF('Post Performance Tracker'!G:G,"Abstract Motion",'Post Performance Tracker'!P:P)</f>
+        <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Week 2</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
+          <t>Pain Point Illustration</t>
+        </is>
+      </c>
+      <c r="B19">
+        <f>COUNTIF('Post Performance Tracker'!G:G,"Pain Point Illustration")</f>
+        <v/>
+      </c>
+      <c r="C19" s="3">
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!G:G,"Pain Point Illustration",'Post Performance Tracker'!S:S),0)</f>
+        <v/>
+      </c>
+      <c r="D19">
+        <f>SUMIF('Post Performance Tracker'!G:G,"Pain Point Illustration",'Post Performance Tracker'!N:N)</f>
+        <v/>
+      </c>
+      <c r="E19">
+        <f>SUMIF('Post Performance Tracker'!G:G,"Pain Point Illustration",'Post Performance Tracker'!P:P)</f>
+        <v/>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Week 3</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
+          <t>Text Overlay</t>
+        </is>
+      </c>
+      <c r="B20">
+        <f>COUNTIF('Post Performance Tracker'!G:G,"Text Overlay")</f>
+        <v/>
+      </c>
+      <c r="C20" s="3">
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!G:G,"Text Overlay",'Post Performance Tracker'!S:S),0)</f>
+        <v/>
+      </c>
+      <c r="D20">
+        <f>SUMIF('Post Performance Tracker'!G:G,"Text Overlay",'Post Performance Tracker'!N:N)</f>
+        <v/>
+      </c>
+      <c r="E20">
+        <f>SUMIF('Post Performance Tracker'!G:G,"Text Overlay",'Post Performance Tracker'!P:P)</f>
+        <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Week 4</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="4" t="inlineStr">
-        <is>
-          <t>CONVERSION FUNNEL</t>
-        </is>
+          <t>Before-After</t>
+        </is>
+      </c>
+      <c r="B21">
+        <f>COUNTIF('Post Performance Tracker'!G:G,"Before-After")</f>
+        <v/>
+      </c>
+      <c r="C21" s="3">
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!G:G,"Before-After",'Post Performance Tracker'!S:S),0)</f>
+        <v/>
+      </c>
+      <c r="D21">
+        <f>SUMIF('Post Performance Tracker'!G:G,"Before-After",'Post Performance Tracker'!N:N)</f>
+        <v/>
+      </c>
+      <c r="E21">
+        <f>SUMIF('Post Performance Tracker'!G:G,"Before-After",'Post Performance Tracker'!P:P)</f>
+        <v/>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="inlineStr">
-        <is>
-          <t>Stage</t>
-        </is>
-      </c>
-      <c r="B24" s="6" t="inlineStr">
-        <is>
-          <t>Count</t>
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t>PAIN POINT PERFORMANCE</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Total Impressions</t>
-        </is>
-      </c>
-      <c r="B25">
-        <f>SUM('Post Performance Tracker'!F:F)</f>
-        <v/>
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>Pain Point</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>Posts Count</t>
+        </is>
+      </c>
+      <c r="C25" s="6" t="inlineStr">
+        <is>
+          <t>Avg Engage%</t>
+        </is>
+      </c>
+      <c r="D25" s="6" t="inlineStr">
+        <is>
+          <t>Demos</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Total Engagement</t>
+          <t>Material Cost Overruns</t>
         </is>
       </c>
       <c r="B26">
-        <f>SUM('Post Performance Tracker'!N:N)</f>
+        <f>COUNTIF('Post Performance Tracker'!D:D,"Material Cost Overruns")</f>
+        <v/>
+      </c>
+      <c r="C26" s="3">
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!D:D,"Material Cost Overruns",'Post Performance Tracker'!S:S),0)</f>
+        <v/>
+      </c>
+      <c r="D26">
+        <f>SUMIF('Post Performance Tracker'!D:D,"Material Cost Overruns",'Post Performance Tracker'!P:P)</f>
         <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>DMs Received</t>
+          <t>Labor Burden Blindness</t>
         </is>
       </c>
       <c r="B27">
-        <f>SUM('Post Performance Tracker'!J:J)</f>
+        <f>COUNTIF('Post Performance Tracker'!D:D,"Labor Burden Blindness")</f>
+        <v/>
+      </c>
+      <c r="C27" s="3">
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!D:D,"Labor Burden Blindness",'Post Performance Tracker'!S:S),0)</f>
+        <v/>
+      </c>
+      <c r="D27">
+        <f>SUMIF('Post Performance Tracker'!D:D,"Labor Burden Blindness",'Post Performance Tracker'!P:P)</f>
         <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Videos Sent</t>
+          <t>Admin Time Waste</t>
         </is>
       </c>
       <c r="B28">
-        <f>SUM('Post Performance Tracker'!K:K)</f>
+        <f>COUNTIF('Post Performance Tracker'!D:D,"Admin Time Waste")</f>
+        <v/>
+      </c>
+      <c r="C28" s="3">
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!D:D,"Admin Time Waste",'Post Performance Tracker'!S:S),0)</f>
+        <v/>
+      </c>
+      <c r="D28">
+        <f>SUMIF('Post Performance Tracker'!D:D,"Admin Time Waste",'Post Performance Tracker'!P:P)</f>
         <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>Cash Flow Delays</t>
+        </is>
+      </c>
+      <c r="B29">
+        <f>COUNTIF('Post Performance Tracker'!D:D,"Cash Flow Delays")</f>
+        <v/>
+      </c>
+      <c r="C29" s="3">
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!D:D,"Cash Flow Delays",'Post Performance Tracker'!S:S),0)</f>
+        <v/>
+      </c>
+      <c r="D29">
+        <f>SUMIF('Post Performance Tracker'!D:D,"Cash Flow Delays",'Post Performance Tracker'!P:P)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Job Profitability Opacity</t>
+        </is>
+      </c>
+      <c r="B30">
+        <f>COUNTIF('Post Performance Tracker'!D:D,"Job Profitability Opacity")</f>
+        <v/>
+      </c>
+      <c r="C30" s="3">
+        <f>IFERROR(AVERAGEIF('Post Performance Tracker'!D:D,"Job Profitability Opacity",'Post Performance Tracker'!S:S),0)</f>
+        <v/>
+      </c>
+      <c r="D30">
+        <f>SUMIF('Post Performance Tracker'!D:D,"Job Profitability Opacity",'Post Performance Tracker'!P:P)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="inlineStr">
+        <is>
+          <t>CONVERSION FUNNEL</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="7" t="inlineStr">
+        <is>
+          <t>Stage</t>
+        </is>
+      </c>
+      <c r="B34" s="7" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Total Impressions</t>
+        </is>
+      </c>
+      <c r="B35">
+        <f>SUM('Post Performance Tracker'!J:J)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Total Engagement</t>
+        </is>
+      </c>
+      <c r="B36">
+        <f>SUM('Post Performance Tracker'!R:R)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>DMs Received</t>
+        </is>
+      </c>
+      <c r="B37">
+        <f>SUM('Post Performance Tracker'!N:N)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Videos Sent</t>
+        </is>
+      </c>
+      <c r="B38">
+        <f>SUM('Post Performance Tracker'!O:O)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
           <t>Demos Booked</t>
         </is>
       </c>
-      <c r="B29">
-        <f>SUM('Post Performance Tracker'!L:L)</f>
+      <c r="B39">
+        <f>SUM('Post Performance Tracker'!P:P)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="5" t="inlineStr">
+        <is>
+          <t>VIDEO ROI SUMMARY</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Total Video Cost</t>
+        </is>
+      </c>
+      <c r="B43" s="4">
+        <f>SUM('Post Performance Tracker'!I:I)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Cost per Demo (Video Posts)</t>
+        </is>
+      </c>
+      <c r="B44" s="4">
+        <f>IF(SUM('Post Performance Tracker'!P:P)&gt;0,B43/SUMIF('Post Performance Tracker'!F:F,"&lt;&gt;None",'Post Performance Tracker'!P:P),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Video Engagement Premium</t>
+        </is>
+      </c>
+      <c r="B45" s="10">
+        <f>IF(C11&gt;0,(C12+C13)/2/C11-1,0)</f>
         <v/>
       </c>
     </row>
@@ -1874,18 +2282,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I100">
-    <cfRule type="cellIs" priority="1" operator="greaterThan" dxfId="4">
+    <cfRule type="cellIs" priority="1" operator="greaterThan" dxfId="6">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L100">
-    <cfRule type="cellIs" priority="2" operator="containsText" dxfId="5">
+    <cfRule type="cellIs" priority="2" operator="containsText" dxfId="7">
       <formula>"Stage 3"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="containsText" dxfId="6">
+    <cfRule type="cellIs" priority="3" operator="containsText" dxfId="8">
       <formula>"Stage 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="containsText" dxfId="7">
+    <cfRule type="cellIs" priority="4" operator="containsText" dxfId="9">
       <formula>"Stage 1"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>